<commit_message>
change pear field name
</commit_message>
<xml_diff>
--- a/src/apps/dailytrans/reports/template.xlsx
+++ b/src/apps/dailytrans/reports/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ai\Desktop\repositories\aprp_on_174\src\apps\dailytrans\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14250E4B-68D7-4DF6-B5AD-B9F53063140B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A491A7-67B5-489A-AEA6-1D090B55662E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-48" yWindow="-48" windowWidth="23136" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="a week" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -462,9 +460,6 @@
   </si>
   <si>
     <t>41-2</t>
-  </si>
-  <si>
-    <t>新興梨</t>
   </si>
   <si>
     <t>41-3</t>
@@ -1480,6 +1475,10 @@
       </rPr>
       <t>台灣地區各縣米穀價格調查日報表，本會農糧署。</t>
     </r>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>新興梨</t>
     <phoneticPr fontId="26" type="noConversion"/>
   </si>
 </sst>
@@ -2042,6 +2041,36 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="180" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="21" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2080,36 +2109,6 @@
     </xf>
     <xf numFmtId="179" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="21" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2198,9 +2197,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2238,9 +2237,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2273,9 +2272,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2308,9 +2324,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2490,32 +2523,32 @@
   <dimension ref="A1:IU257"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="70" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A136" sqref="A136"/>
+      <pane ySplit="8" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="22.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="6.62890625" customWidth="1"/>
-    <col min="2" max="2" width="6.62890625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.625" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3671875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1015625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="9.62890625" customWidth="1"/>
-    <col min="7" max="7" width="10.734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.62890625" style="3" customWidth="1"/>
-    <col min="9" max="11" width="7.89453125" style="3" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="8.734375" style="3" customWidth="1"/>
-    <col min="13" max="19" width="8.62890625" style="4" customWidth="1"/>
-    <col min="20" max="20" width="21.47265625" customWidth="1"/>
-    <col min="21" max="21" width="11.3671875" customWidth="1"/>
-    <col min="22" max="22" width="4.89453125" customWidth="1"/>
-    <col min="23" max="23" width="10.62890625" hidden="1" customWidth="1"/>
-    <col min="24" max="30" width="14.47265625" hidden="1" customWidth="1"/>
-    <col min="31" max="46" width="5.62890625" customWidth="1"/>
+    <col min="4" max="4" width="10.375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" customWidth="1"/>
+    <col min="7" max="7" width="10.75" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.625" style="3" customWidth="1"/>
+    <col min="9" max="11" width="7.875" style="3" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.75" style="3" customWidth="1"/>
+    <col min="13" max="19" width="8.625" style="4" customWidth="1"/>
+    <col min="20" max="20" width="21.5" customWidth="1"/>
+    <col min="21" max="21" width="11.375" customWidth="1"/>
+    <col min="22" max="22" width="4.875" customWidth="1"/>
+    <col min="23" max="23" width="10.625" hidden="1" customWidth="1"/>
+    <col min="24" max="30" width="14.5" hidden="1" customWidth="1"/>
+    <col min="31" max="46" width="5.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="11.5" customHeight="1">
+    <row r="1" spans="1:30" ht="11.45" customHeight="1">
       <c r="A1" s="5"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -2524,37 +2557,37 @@
       <c r="F1" s="7"/>
       <c r="G1" s="8"/>
       <c r="H1" s="9"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:30" s="10" customFormat="1" ht="51" customHeight="1">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
-      <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-    </row>
-    <row r="3" spans="1:30" ht="11.5" customHeight="1">
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+    </row>
+    <row r="3" spans="1:30" ht="11.45" customHeight="1">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -2592,7 +2625,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
     </row>
-    <row r="5" spans="1:30" ht="40" customHeight="1">
+    <row r="5" spans="1:30" ht="39.950000000000003" customHeight="1">
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="16"/>
@@ -2601,8 +2634,8 @@
       <c r="G5" s="18"/>
       <c r="H5" s="19"/>
       <c r="I5" s="20"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
       <c r="L5" s="19"/>
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
@@ -2611,41 +2644,41 @@
       <c r="S5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="T5" s="75" t="s">
+      <c r="T5" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="75"/>
+      <c r="U5" s="85"/>
     </row>
     <row r="6" spans="1:30" s="10" customFormat="1" ht="31.9" customHeight="1">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="79" t="s">
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="80" t="s">
+      <c r="G6" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="76" t="s">
+      <c r="H6" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="76"/>
-      <c r="R6" s="76"/>
-      <c r="S6" s="76"/>
-      <c r="T6" s="76"/>
-      <c r="U6" s="76"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+      <c r="N6" s="86"/>
+      <c r="O6" s="86"/>
+      <c r="P6" s="86"/>
+      <c r="Q6" s="86"/>
+      <c r="R6" s="86"/>
+      <c r="S6" s="86"/>
+      <c r="T6" s="86"/>
+      <c r="U6" s="86"/>
       <c r="V6"/>
       <c r="W6" s="26"/>
       <c r="X6" s="26"/>
@@ -2656,37 +2689,37 @@
       <c r="AC6" s="26"/>
       <c r="AD6" s="26"/>
     </row>
-    <row r="7" spans="1:30" s="10" customFormat="1" ht="50.5" customHeight="1">
-      <c r="A7" s="76"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="78"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="81" t="s">
+    <row r="7" spans="1:30" s="10" customFormat="1" ht="50.45" customHeight="1">
+      <c r="A7" s="86"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="90"/>
+      <c r="H7" s="91" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
       <c r="K7" s="27"/>
-      <c r="L7" s="82" t="s">
-        <v>245</v>
-      </c>
-      <c r="M7" s="83" t="s">
+      <c r="L7" s="92" t="s">
+        <v>244</v>
+      </c>
+      <c r="M7" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="83"/>
-      <c r="O7" s="83"/>
-      <c r="P7" s="83"/>
-      <c r="Q7" s="83"/>
-      <c r="R7" s="83"/>
-      <c r="S7" s="83"/>
-      <c r="T7" s="84" t="s">
+      <c r="N7" s="93"/>
+      <c r="O7" s="93"/>
+      <c r="P7" s="93"/>
+      <c r="Q7" s="93"/>
+      <c r="R7" s="93"/>
+      <c r="S7" s="93"/>
+      <c r="T7" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="U7" s="84"/>
-      <c r="V7" s="85"/>
+      <c r="U7" s="94"/>
+      <c r="V7" s="79"/>
       <c r="W7" s="28"/>
       <c r="X7" s="28"/>
       <c r="Y7" s="28"/>
@@ -2697,14 +2730,14 @@
       <c r="AD7" s="28"/>
     </row>
     <row r="8" spans="1:30" s="10" customFormat="1" ht="49.5">
-      <c r="A8" s="76"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="80"/>
-      <c r="H8" s="81"/>
+      <c r="A8" s="86"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="91"/>
       <c r="I8" s="29" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -2717,9 +2750,9 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L8" s="82"/>
+      <c r="L8" s="92"/>
       <c r="M8" s="30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N8" s="30" t="s">
         <v>10</v>
@@ -2743,9 +2776,9 @@
         <v>11</v>
       </c>
       <c r="U8" s="31" t="s">
-        <v>247</v>
-      </c>
-      <c r="V8" s="85"/>
+        <v>246</v>
+      </c>
+      <c r="V8" s="79"/>
       <c r="W8" s="32" t="s">
         <v>12</v>
       </c>
@@ -2771,17 +2804,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="9" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A9" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="86"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="88" t="s">
+      <c r="C9" s="72"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="81" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="35" t="s">
@@ -2854,17 +2887,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="10" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A10" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="86"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="87"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
       <c r="G10" s="35" t="s">
         <v>15</v>
       </c>
@@ -2935,14 +2968,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="11" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A11" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="86"/>
+      <c r="C11" s="72"/>
       <c r="D11" s="34" t="s">
         <v>15</v>
       </c>
@@ -3022,14 +3055,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="12" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A12" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="72" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="86"/>
+      <c r="C12" s="72"/>
       <c r="D12" s="34" t="s">
         <v>15</v>
       </c>
@@ -3109,14 +3142,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="13" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A13" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="86"/>
+      <c r="C13" s="72"/>
       <c r="D13" s="34" t="s">
         <v>15</v>
       </c>
@@ -3196,14 +3229,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="14" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A14" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="89" t="s">
+      <c r="B14" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="89"/>
+      <c r="C14" s="73"/>
       <c r="D14" s="41"/>
       <c r="E14" s="41"/>
       <c r="F14" s="34" t="s">
@@ -3280,14 +3313,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="15" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A15" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="89" t="s">
+      <c r="B15" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="89"/>
+      <c r="C15" s="73"/>
       <c r="D15" s="41"/>
       <c r="E15" s="41"/>
       <c r="F15" s="34" t="s">
@@ -3363,14 +3396,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="16" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A16" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="89" t="s">
+      <c r="B16" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="89"/>
+      <c r="C16" s="73"/>
       <c r="D16" s="41"/>
       <c r="E16" s="41"/>
       <c r="F16" s="34" t="s">
@@ -3446,14 +3479,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="17" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A17" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="89" t="s">
+      <c r="B17" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="89"/>
+      <c r="C17" s="73"/>
       <c r="D17" s="41"/>
       <c r="E17" s="41"/>
       <c r="F17" s="34" t="s">
@@ -3529,14 +3562,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="18" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A18" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="90" t="s">
+      <c r="B18" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="90"/>
+      <c r="C18" s="78"/>
       <c r="D18" s="41"/>
       <c r="E18" s="41"/>
       <c r="F18" s="34" t="s">
@@ -3612,14 +3645,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="19" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A19" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="89" t="s">
+      <c r="B19" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="89"/>
+      <c r="C19" s="73"/>
       <c r="D19" s="41"/>
       <c r="E19" s="41"/>
       <c r="F19" s="34" t="s">
@@ -3695,14 +3728,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="20" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A20" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="89" t="s">
+      <c r="B20" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="89"/>
+      <c r="C20" s="73"/>
       <c r="D20" s="41"/>
       <c r="E20" s="41"/>
       <c r="F20" s="34" t="s">
@@ -3778,14 +3811,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="21" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A21" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="89" t="s">
+      <c r="B21" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="89"/>
+      <c r="C21" s="73"/>
       <c r="D21" s="41"/>
       <c r="E21" s="41"/>
       <c r="F21" s="34" t="s">
@@ -3861,14 +3894,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="22" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A22" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="89" t="s">
+      <c r="B22" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="89"/>
+      <c r="C22" s="73"/>
       <c r="D22" s="41"/>
       <c r="E22" s="41"/>
       <c r="F22" s="34" t="s">
@@ -3948,10 +3981,10 @@
       <c r="A23" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="89" t="s">
+      <c r="B23" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="89"/>
+      <c r="C23" s="73"/>
       <c r="D23" s="41"/>
       <c r="E23" s="41"/>
       <c r="F23" s="34" t="s">
@@ -4027,14 +4060,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="24" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A24" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="89" t="s">
+      <c r="B24" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="89"/>
+      <c r="C24" s="73"/>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
       <c r="F24" s="34" t="s">
@@ -4110,14 +4143,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="25" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A25" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="90" t="s">
+      <c r="B25" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="90"/>
+      <c r="C25" s="78"/>
       <c r="D25" s="41"/>
       <c r="E25" s="41"/>
       <c r="F25" s="34" t="s">
@@ -4193,14 +4226,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="26" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A26" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="89" t="s">
+      <c r="B26" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="89"/>
+      <c r="C26" s="73"/>
       <c r="D26" s="41"/>
       <c r="E26" s="41"/>
       <c r="F26" s="34" t="s">
@@ -4276,14 +4309,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="27" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A27" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="89"/>
+      <c r="C27" s="73"/>
       <c r="D27" s="41"/>
       <c r="E27" s="41"/>
       <c r="F27" s="34" t="s">
@@ -4359,14 +4392,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="28" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A28" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="89" t="s">
+      <c r="B28" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="89"/>
+      <c r="C28" s="73"/>
       <c r="D28" s="41"/>
       <c r="E28" s="41"/>
       <c r="F28" s="34" t="s">
@@ -4442,14 +4475,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="29" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A29" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="90" t="s">
+      <c r="B29" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="90"/>
+      <c r="C29" s="78"/>
       <c r="D29" s="41"/>
       <c r="E29" s="41"/>
       <c r="F29" s="34" t="s">
@@ -4526,14 +4559,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="30" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A30" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="90" t="s">
+      <c r="B30" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="90"/>
+      <c r="C30" s="78"/>
       <c r="D30" s="41"/>
       <c r="E30" s="41"/>
       <c r="F30" s="34" t="s">
@@ -4610,14 +4643,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="31" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A31" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="89" t="s">
+      <c r="B31" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="89"/>
+      <c r="C31" s="73"/>
       <c r="D31" s="41"/>
       <c r="E31" s="41"/>
       <c r="F31" s="34" t="s">
@@ -4693,14 +4726,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="32" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A32" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="89" t="s">
+      <c r="B32" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="89"/>
+      <c r="C32" s="73"/>
       <c r="D32" s="41"/>
       <c r="E32" s="41"/>
       <c r="F32" s="34" t="s">
@@ -4776,14 +4809,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="33" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A33" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="89" t="s">
+      <c r="B33" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="89"/>
+      <c r="C33" s="73"/>
       <c r="D33" s="43"/>
       <c r="E33" s="43"/>
       <c r="F33" s="34" t="s">
@@ -4860,14 +4893,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="34" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A34" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="89" t="s">
+      <c r="B34" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="89"/>
+      <c r="C34" s="73"/>
       <c r="D34" s="43"/>
       <c r="E34" s="43"/>
       <c r="F34" s="34" t="s">
@@ -4943,14 +4976,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="35" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A35" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="89" t="s">
+      <c r="B35" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="89"/>
+      <c r="C35" s="73"/>
       <c r="D35" s="43"/>
       <c r="E35" s="43"/>
       <c r="F35" s="34" t="s">
@@ -5026,14 +5059,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="36" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A36" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="89" t="s">
+      <c r="B36" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="89"/>
+      <c r="C36" s="73"/>
       <c r="D36" s="43"/>
       <c r="E36" s="43"/>
       <c r="F36" s="34" t="s">
@@ -5109,14 +5142,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="37" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A37" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="89" t="s">
+      <c r="B37" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="89"/>
+      <c r="C37" s="73"/>
       <c r="D37" s="43"/>
       <c r="E37" s="43"/>
       <c r="F37" s="34" t="s">
@@ -5192,14 +5225,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="38" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A38" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="89" t="s">
+      <c r="B38" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="89"/>
+      <c r="C38" s="73"/>
       <c r="D38" s="43"/>
       <c r="E38" s="43"/>
       <c r="F38" s="34" t="s">
@@ -5275,14 +5308,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="39" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A39" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="89" t="s">
+      <c r="B39" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="89"/>
+      <c r="C39" s="73"/>
       <c r="D39" s="43"/>
       <c r="E39" s="43"/>
       <c r="F39" s="34" t="s">
@@ -5358,14 +5391,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="40" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A40" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="89" t="s">
+      <c r="B40" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="89"/>
+      <c r="C40" s="73"/>
       <c r="D40" s="43"/>
       <c r="E40" s="43"/>
       <c r="F40" s="34" t="s">
@@ -5441,14 +5474,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="41" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A41" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="89" t="s">
+      <c r="B41" s="73" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="89"/>
+      <c r="C41" s="73"/>
       <c r="D41" s="43"/>
       <c r="E41" s="43"/>
       <c r="F41" s="34" t="s">
@@ -5524,14 +5557,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="42" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A42" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="89" t="s">
+      <c r="B42" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="89"/>
+      <c r="C42" s="73"/>
       <c r="D42" s="43"/>
       <c r="E42" s="43"/>
       <c r="F42" s="34" t="s">
@@ -5608,14 +5641,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="43" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A43" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="91" t="s">
+      <c r="B43" s="77" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="91"/>
+      <c r="C43" s="77"/>
       <c r="D43" s="43"/>
       <c r="E43" s="43"/>
       <c r="F43" s="34" t="s">
@@ -5691,14 +5724,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="44" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A44" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="91" t="s">
+      <c r="B44" s="77" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="91"/>
+      <c r="C44" s="77"/>
       <c r="D44" s="43"/>
       <c r="E44" s="43"/>
       <c r="F44" s="34" t="s">
@@ -5774,14 +5807,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="45" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A45" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="89" t="s">
+      <c r="B45" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="89"/>
+      <c r="C45" s="73"/>
       <c r="D45" s="43"/>
       <c r="E45" s="43"/>
       <c r="F45" s="34" t="s">
@@ -5857,14 +5890,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="46" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A46" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="89" t="s">
+      <c r="B46" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="89"/>
+      <c r="C46" s="73"/>
       <c r="D46" s="43"/>
       <c r="E46" s="43"/>
       <c r="F46" s="34" t="s">
@@ -5940,14 +5973,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="47" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A47" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="89" t="s">
+      <c r="B47" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="89"/>
+      <c r="C47" s="73"/>
       <c r="D47" s="43"/>
       <c r="E47" s="43"/>
       <c r="F47" s="34" t="s">
@@ -6023,14 +6056,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="48" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A48" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="89" t="s">
+      <c r="B48" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="89"/>
+      <c r="C48" s="73"/>
       <c r="D48" s="43"/>
       <c r="E48" s="43"/>
       <c r="F48" s="34" t="s">
@@ -6106,14 +6139,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="49" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A49" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="89" t="s">
+      <c r="B49" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="89"/>
+      <c r="C49" s="73"/>
       <c r="D49" s="43"/>
       <c r="E49" s="43"/>
       <c r="F49" s="34" t="s">
@@ -6189,14 +6222,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="50" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A50" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="89" t="s">
+      <c r="B50" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="89"/>
+      <c r="C50" s="73"/>
       <c r="D50" s="43"/>
       <c r="E50" s="43"/>
       <c r="F50" s="34" t="s">
@@ -6272,14 +6305,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="51" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A51" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="89" t="s">
+      <c r="B51" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="89"/>
+      <c r="C51" s="73"/>
       <c r="D51" s="43"/>
       <c r="E51" s="43"/>
       <c r="F51" s="34" t="s">
@@ -6355,14 +6388,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="52" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A52" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="89" t="s">
+      <c r="B52" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="89"/>
+      <c r="C52" s="73"/>
       <c r="D52" s="43"/>
       <c r="E52" s="43"/>
       <c r="F52" s="34" t="s">
@@ -6438,14 +6471,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="53" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A53" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="89" t="s">
+      <c r="B53" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="89"/>
+      <c r="C53" s="73"/>
       <c r="D53" s="43"/>
       <c r="E53" s="43"/>
       <c r="F53" s="34" t="s">
@@ -6521,14 +6554,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="54" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A54" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="89" t="s">
+      <c r="B54" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="89"/>
+      <c r="C54" s="73"/>
       <c r="D54" s="43"/>
       <c r="E54" s="43"/>
       <c r="F54" s="34" t="s">
@@ -6604,14 +6637,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="55" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A55" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="89" t="s">
+      <c r="B55" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C55" s="89"/>
+      <c r="C55" s="73"/>
       <c r="D55" s="43"/>
       <c r="E55" s="43"/>
       <c r="F55" s="34" t="s">
@@ -6687,14 +6720,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="56" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A56" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="B56" s="89" t="s">
+      <c r="B56" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="89"/>
+      <c r="C56" s="73"/>
       <c r="D56" s="43"/>
       <c r="E56" s="43"/>
       <c r="F56" s="34" t="s">
@@ -6770,14 +6803,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="57" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A57" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="89" t="s">
-        <v>102</v>
-      </c>
-      <c r="C57" s="89"/>
+      <c r="B57" s="73" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="73"/>
       <c r="D57" s="43"/>
       <c r="E57" s="43"/>
       <c r="F57" s="34" t="s">
@@ -6853,14 +6886,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:30" s="44" customFormat="1" ht="38.5" customHeight="1">
+    <row r="58" spans="1:30" s="44" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A58" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="B58" s="89" t="s">
-        <v>104</v>
-      </c>
-      <c r="C58" s="89"/>
+        <v>102</v>
+      </c>
+      <c r="B58" s="73" t="s">
+        <v>255</v>
+      </c>
+      <c r="C58" s="73"/>
       <c r="D58" s="43"/>
       <c r="E58" s="43"/>
       <c r="F58" s="34" t="s">
@@ -6936,14 +6969,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="59" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A59" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" s="73" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="89" t="s">
-        <v>106</v>
-      </c>
-      <c r="C59" s="89"/>
+      <c r="C59" s="73"/>
       <c r="D59" s="43"/>
       <c r="E59" s="43"/>
       <c r="F59" s="34" t="s">
@@ -7019,14 +7052,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="60" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A60" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B60" s="73" t="s">
         <v>107</v>
       </c>
-      <c r="B60" s="89" t="s">
-        <v>108</v>
-      </c>
-      <c r="C60" s="89"/>
+      <c r="C60" s="73"/>
       <c r="D60" s="43"/>
       <c r="E60" s="43"/>
       <c r="F60" s="34" t="s">
@@ -7102,14 +7135,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="61" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A61" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B61" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="B61" s="89" t="s">
-        <v>110</v>
-      </c>
-      <c r="C61" s="89"/>
+      <c r="C61" s="73"/>
       <c r="D61" s="43"/>
       <c r="E61" s="43"/>
       <c r="F61" s="34" t="s">
@@ -7185,14 +7218,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="62" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A62" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="B62" s="73" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="89" t="s">
-        <v>112</v>
-      </c>
-      <c r="C62" s="89"/>
+      <c r="C62" s="73"/>
       <c r="D62" s="43"/>
       <c r="E62" s="43"/>
       <c r="F62" s="34" t="s">
@@ -7269,14 +7302,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="63" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A63" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="B63" s="89" t="s">
-        <v>250</v>
-      </c>
-      <c r="C63" s="89"/>
+        <v>112</v>
+      </c>
+      <c r="B63" s="73" t="s">
+        <v>249</v>
+      </c>
+      <c r="C63" s="73"/>
       <c r="D63" s="43"/>
       <c r="E63" s="43"/>
       <c r="F63" s="34" t="s">
@@ -7352,14 +7385,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="64" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A64" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B64" s="73" t="s">
         <v>114</v>
       </c>
-      <c r="B64" s="89" t="s">
-        <v>115</v>
-      </c>
-      <c r="C64" s="89"/>
+      <c r="C64" s="73"/>
       <c r="D64" s="43"/>
       <c r="E64" s="43"/>
       <c r="F64" s="34" t="s">
@@ -7436,14 +7469,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="65" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A65" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="B65" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="89" t="s">
-        <v>117</v>
-      </c>
-      <c r="C65" s="89"/>
+      <c r="C65" s="73"/>
       <c r="D65" s="43"/>
       <c r="E65" s="43"/>
       <c r="F65" s="34" t="s">
@@ -7519,14 +7552,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="66" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A66" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="B66" s="73" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="89" t="s">
-        <v>119</v>
-      </c>
-      <c r="C66" s="89"/>
+      <c r="C66" s="73"/>
       <c r="D66" s="43"/>
       <c r="E66" s="43"/>
       <c r="F66" s="34" t="s">
@@ -7603,14 +7636,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="67" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A67" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B67" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="89" t="s">
-        <v>121</v>
-      </c>
-      <c r="C67" s="89"/>
+      <c r="C67" s="73"/>
       <c r="D67" s="43"/>
       <c r="E67" s="43"/>
       <c r="F67" s="34" t="s">
@@ -7686,14 +7719,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="68" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A68" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="B68" s="73" t="s">
         <v>122</v>
       </c>
-      <c r="B68" s="89" t="s">
-        <v>123</v>
-      </c>
-      <c r="C68" s="89"/>
+      <c r="C68" s="73"/>
       <c r="D68" s="43"/>
       <c r="E68" s="43"/>
       <c r="F68" s="34" t="s">
@@ -7769,14 +7802,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="69" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A69" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="B69" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="B69" s="89" t="s">
-        <v>125</v>
-      </c>
-      <c r="C69" s="89"/>
+      <c r="C69" s="73"/>
       <c r="D69" s="43"/>
       <c r="E69" s="43"/>
       <c r="F69" s="34" t="s">
@@ -7853,14 +7886,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="70" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A70" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="73" t="s">
         <v>126</v>
       </c>
-      <c r="B70" s="89" t="s">
-        <v>127</v>
-      </c>
-      <c r="C70" s="89"/>
+      <c r="C70" s="73"/>
       <c r="D70" s="43"/>
       <c r="E70" s="43"/>
       <c r="F70" s="34" t="s">
@@ -7936,14 +7969,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="71" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A71" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="B71" s="75" t="s">
         <v>128</v>
       </c>
-      <c r="B71" s="92" t="s">
-        <v>129</v>
-      </c>
-      <c r="C71" s="92"/>
+      <c r="C71" s="75"/>
       <c r="D71" s="45"/>
       <c r="E71" s="45"/>
       <c r="F71" s="34" t="s">
@@ -8020,12 +8053,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="72" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A72" s="46"/>
-      <c r="B72" s="89" t="s">
-        <v>130</v>
-      </c>
-      <c r="C72" s="89"/>
+      <c r="B72" s="73" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="73"/>
       <c r="D72" s="43"/>
       <c r="E72" s="43"/>
       <c r="F72" s="34" t="s">
@@ -8102,16 +8135,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="73" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A73" s="38"/>
-      <c r="B73" s="93" t="s">
-        <v>131</v>
-      </c>
-      <c r="C73" s="93"/>
-      <c r="D73" s="93">
+      <c r="B73" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="C73" s="76"/>
+      <c r="D73" s="76">
         <v>35.200000000000003</v>
       </c>
-      <c r="E73" s="93"/>
+      <c r="E73" s="76"/>
       <c r="F73" s="34" t="s">
         <v>15</v>
       </c>
@@ -8185,14 +8218,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="74" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A74" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B74" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="B74" s="89" t="s">
-        <v>133</v>
-      </c>
-      <c r="C74" s="89"/>
+      <c r="C74" s="73"/>
       <c r="D74" s="43"/>
       <c r="E74" s="43"/>
       <c r="F74" s="34" t="s">
@@ -8268,14 +8301,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="75" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="75" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A75" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B75" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="B75" s="89" t="s">
-        <v>135</v>
-      </c>
-      <c r="C75" s="89"/>
+      <c r="C75" s="73"/>
       <c r="D75" s="43"/>
       <c r="E75" s="43"/>
       <c r="F75" s="34" t="s">
@@ -8351,14 +8384,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="76" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A76" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B76" s="73" t="s">
         <v>136</v>
       </c>
-      <c r="B76" s="89" t="s">
-        <v>137</v>
-      </c>
-      <c r="C76" s="89"/>
+      <c r="C76" s="73"/>
       <c r="D76" s="43"/>
       <c r="E76" s="43"/>
       <c r="F76" s="34" t="s">
@@ -8435,14 +8468,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="77" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A77" s="33">
         <v>0</v>
       </c>
-      <c r="B77" s="89" t="s">
-        <v>138</v>
-      </c>
-      <c r="C77" s="89"/>
+      <c r="B77" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="C77" s="73"/>
       <c r="D77" s="43"/>
       <c r="E77" s="43"/>
       <c r="F77" s="34" t="s">
@@ -8518,14 +8551,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="78" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A78" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B78" s="73" t="s">
         <v>139</v>
       </c>
-      <c r="B78" s="89" t="s">
-        <v>140</v>
-      </c>
-      <c r="C78" s="89"/>
+      <c r="C78" s="73"/>
       <c r="D78" s="43"/>
       <c r="E78" s="43"/>
       <c r="F78" s="34" t="s">
@@ -8601,14 +8634,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="79" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A79" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B79" s="73" t="s">
         <v>141</v>
       </c>
-      <c r="B79" s="89" t="s">
-        <v>142</v>
-      </c>
-      <c r="C79" s="89"/>
+      <c r="C79" s="73"/>
       <c r="D79" s="43"/>
       <c r="E79" s="43"/>
       <c r="F79" s="34" t="s">
@@ -8684,14 +8717,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="80" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A80" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="B80" s="89" t="s">
-        <v>253</v>
-      </c>
-      <c r="C80" s="89"/>
+        <v>142</v>
+      </c>
+      <c r="B80" s="73" t="s">
+        <v>252</v>
+      </c>
+      <c r="C80" s="73"/>
       <c r="D80" s="43"/>
       <c r="E80" s="43"/>
       <c r="F80" s="34" t="s">
@@ -8767,14 +8800,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="81" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A81" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="B81" s="73" t="s">
         <v>144</v>
       </c>
-      <c r="B81" s="89" t="s">
-        <v>145</v>
-      </c>
-      <c r="C81" s="89"/>
+      <c r="C81" s="73"/>
       <c r="D81" s="43"/>
       <c r="E81" s="43"/>
       <c r="F81" s="34" t="s">
@@ -8850,14 +8883,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="82" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A82" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="B82" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="B82" s="89" t="s">
-        <v>147</v>
-      </c>
-      <c r="C82" s="89"/>
+      <c r="C82" s="73"/>
       <c r="D82" s="43"/>
       <c r="E82" s="43"/>
       <c r="F82" s="34" t="s">
@@ -8934,14 +8967,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="83" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A83" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B83" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="B83" s="89" t="s">
-        <v>149</v>
-      </c>
-      <c r="C83" s="89"/>
+      <c r="C83" s="73"/>
       <c r="D83" s="43"/>
       <c r="E83" s="43"/>
       <c r="F83" s="34" t="s">
@@ -9018,14 +9051,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="84" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A84" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B84" s="73" t="s">
         <v>150</v>
       </c>
-      <c r="B84" s="89" t="s">
-        <v>151</v>
-      </c>
-      <c r="C84" s="89"/>
+      <c r="C84" s="73"/>
       <c r="D84" s="43"/>
       <c r="E84" s="43"/>
       <c r="F84" s="34" t="s">
@@ -9102,14 +9135,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="85" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="85" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A85" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B85" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="B85" s="89" t="s">
-        <v>153</v>
-      </c>
-      <c r="C85" s="89"/>
+      <c r="C85" s="73"/>
       <c r="D85" s="43"/>
       <c r="E85" s="43"/>
       <c r="F85" s="34" t="s">
@@ -9186,14 +9219,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="86" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A86" s="33" t="s">
+        <v>153</v>
+      </c>
+      <c r="B86" s="73" t="s">
         <v>154</v>
       </c>
-      <c r="B86" s="89" t="s">
-        <v>155</v>
-      </c>
-      <c r="C86" s="89"/>
+      <c r="C86" s="73"/>
       <c r="D86" s="43"/>
       <c r="E86" s="43"/>
       <c r="F86" s="34" t="s">
@@ -9270,14 +9303,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="87" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A87" s="33" t="s">
+        <v>155</v>
+      </c>
+      <c r="B87" s="73" t="s">
         <v>156</v>
       </c>
-      <c r="B87" s="89" t="s">
-        <v>157</v>
-      </c>
-      <c r="C87" s="89"/>
+      <c r="C87" s="73"/>
       <c r="D87" s="43"/>
       <c r="E87" s="43"/>
       <c r="F87" s="34" t="s">
@@ -9354,14 +9387,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="88" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A88" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="B88" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="B88" s="89" t="s">
-        <v>159</v>
-      </c>
-      <c r="C88" s="89"/>
+      <c r="C88" s="73"/>
       <c r="D88" s="43"/>
       <c r="E88" s="43"/>
       <c r="F88" s="34" t="s">
@@ -9437,14 +9470,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="89" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A89" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="B89" s="73" t="s">
         <v>160</v>
       </c>
-      <c r="B89" s="89" t="s">
-        <v>161</v>
-      </c>
-      <c r="C89" s="89"/>
+      <c r="C89" s="73"/>
       <c r="D89" s="43"/>
       <c r="E89" s="43"/>
       <c r="F89" s="34" t="s">
@@ -9520,14 +9553,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="90" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A90" s="33" t="s">
-        <v>162</v>
-      </c>
-      <c r="B90" s="89" t="s">
-        <v>251</v>
-      </c>
-      <c r="C90" s="89"/>
+        <v>161</v>
+      </c>
+      <c r="B90" s="73" t="s">
+        <v>250</v>
+      </c>
+      <c r="C90" s="73"/>
       <c r="D90" s="43"/>
       <c r="E90" s="43"/>
       <c r="F90" s="34" t="s">
@@ -9603,14 +9636,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="91" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A91" s="33" t="s">
-        <v>163</v>
-      </c>
-      <c r="B91" s="89" t="s">
+        <v>162</v>
+      </c>
+      <c r="B91" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="89"/>
+      <c r="C91" s="73"/>
       <c r="D91" s="43"/>
       <c r="E91" s="43"/>
       <c r="F91" s="34" t="s">
@@ -9686,14 +9719,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="92" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A92" s="33" t="s">
-        <v>164</v>
-      </c>
-      <c r="B92" s="89" t="s">
+        <v>163</v>
+      </c>
+      <c r="B92" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C92" s="89"/>
+      <c r="C92" s="73"/>
       <c r="D92" s="43"/>
       <c r="E92" s="43"/>
       <c r="F92" s="34" t="s">
@@ -9769,14 +9802,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="93" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A93" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="B93" s="89" t="s">
+        <v>164</v>
+      </c>
+      <c r="B93" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C93" s="89"/>
+      <c r="C93" s="73"/>
       <c r="D93" s="43"/>
       <c r="E93" s="43"/>
       <c r="F93" s="34" t="s">
@@ -9852,14 +9885,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="94" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A94" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="B94" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="B94" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C94" s="89"/>
+      <c r="C94" s="73"/>
       <c r="D94" s="43"/>
       <c r="E94" s="43"/>
       <c r="F94" s="34" t="s">
@@ -9935,14 +9968,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="95" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A95" s="33" t="s">
-        <v>167</v>
-      </c>
-      <c r="B95" s="89" t="s">
+        <v>166</v>
+      </c>
+      <c r="B95" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C95" s="89"/>
+      <c r="C95" s="73"/>
       <c r="D95" s="43"/>
       <c r="E95" s="43"/>
       <c r="F95" s="34" t="s">
@@ -10018,14 +10051,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="96" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="96" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A96" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="B96" s="89" t="s">
+        <v>167</v>
+      </c>
+      <c r="B96" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C96" s="89"/>
+      <c r="C96" s="73"/>
       <c r="D96" s="43"/>
       <c r="E96" s="43"/>
       <c r="F96" s="34" t="s">
@@ -10101,14 +10134,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="97" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="97" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A97" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="B97" s="89" t="s">
+        <v>168</v>
+      </c>
+      <c r="B97" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C97" s="89"/>
+      <c r="C97" s="73"/>
       <c r="D97" s="43"/>
       <c r="E97" s="43"/>
       <c r="F97" s="34" t="s">
@@ -10184,14 +10217,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="98" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A98" s="33" t="s">
-        <v>170</v>
-      </c>
-      <c r="B98" s="89" t="s">
+        <v>169</v>
+      </c>
+      <c r="B98" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="C98" s="89"/>
+      <c r="C98" s="73"/>
       <c r="D98" s="43"/>
       <c r="E98" s="43"/>
       <c r="F98" s="34" t="s">
@@ -10267,14 +10300,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="99" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A99" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="B99" s="73" t="s">
         <v>171</v>
       </c>
-      <c r="B99" s="89" t="s">
-        <v>172</v>
-      </c>
-      <c r="C99" s="89"/>
+      <c r="C99" s="73"/>
       <c r="D99" s="43"/>
       <c r="E99" s="43"/>
       <c r="F99" s="34" t="s">
@@ -10350,14 +10383,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="100" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A100" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="B100" s="73" t="s">
         <v>173</v>
       </c>
-      <c r="B100" s="89" t="s">
-        <v>174</v>
-      </c>
-      <c r="C100" s="89"/>
+      <c r="C100" s="73"/>
       <c r="D100" s="43"/>
       <c r="E100" s="43"/>
       <c r="F100" s="34" t="s">
@@ -10433,14 +10466,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="101" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A101" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="B101" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="B101" s="94" t="s">
-        <v>176</v>
-      </c>
-      <c r="C101" s="94"/>
+      <c r="C101" s="74"/>
       <c r="D101" s="43"/>
       <c r="E101" s="43"/>
       <c r="F101" s="34" t="s">
@@ -10516,14 +10549,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="102" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A102" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="B102" s="73" t="s">
         <v>177</v>
       </c>
-      <c r="B102" s="89" t="s">
-        <v>178</v>
-      </c>
-      <c r="C102" s="89"/>
+      <c r="C102" s="73"/>
       <c r="D102" s="43"/>
       <c r="E102" s="43"/>
       <c r="F102" s="34" t="s">
@@ -10599,14 +10632,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="103" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="103" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A103" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="B103" s="73" t="s">
         <v>179</v>
       </c>
-      <c r="B103" s="89" t="s">
-        <v>180</v>
-      </c>
-      <c r="C103" s="89"/>
+      <c r="C103" s="73"/>
       <c r="D103" s="43"/>
       <c r="E103" s="43"/>
       <c r="F103" s="34" t="s">
@@ -10682,14 +10715,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="104" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A104" s="33" t="s">
+        <v>180</v>
+      </c>
+      <c r="B104" s="73" t="s">
         <v>181</v>
       </c>
-      <c r="B104" s="89" t="s">
-        <v>182</v>
-      </c>
-      <c r="C104" s="89"/>
+      <c r="C104" s="73"/>
       <c r="D104" s="43"/>
       <c r="E104" s="43"/>
       <c r="F104" s="34" t="s">
@@ -10765,14 +10798,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="105" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="105" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A105" s="33" t="s">
+        <v>182</v>
+      </c>
+      <c r="B105" s="73" t="s">
         <v>183</v>
       </c>
-      <c r="B105" s="89" t="s">
-        <v>184</v>
-      </c>
-      <c r="C105" s="89"/>
+      <c r="C105" s="73"/>
       <c r="D105" s="43"/>
       <c r="E105" s="43"/>
       <c r="F105" s="34" t="s">
@@ -10848,14 +10881,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="106" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A106" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B106" s="73" t="s">
         <v>185</v>
       </c>
-      <c r="B106" s="89" t="s">
-        <v>186</v>
-      </c>
-      <c r="C106" s="89"/>
+      <c r="C106" s="73"/>
       <c r="D106" s="43"/>
       <c r="E106" s="43"/>
       <c r="F106" s="34" t="s">
@@ -10931,14 +10964,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="107" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A107" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B107" s="73" t="s">
         <v>187</v>
       </c>
-      <c r="B107" s="89" t="s">
-        <v>188</v>
-      </c>
-      <c r="C107" s="89"/>
+      <c r="C107" s="73"/>
       <c r="D107" s="43"/>
       <c r="E107" s="43"/>
       <c r="F107" s="34" t="s">
@@ -11014,14 +11047,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="108" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A108" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B108" s="74" t="s">
         <v>189</v>
       </c>
-      <c r="B108" s="94" t="s">
-        <v>190</v>
-      </c>
-      <c r="C108" s="94"/>
+      <c r="C108" s="74"/>
       <c r="D108" s="43"/>
       <c r="E108" s="43"/>
       <c r="F108" s="34" t="s">
@@ -11097,14 +11130,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="109" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="109" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A109" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="B109" s="94" t="s">
         <v>190</v>
       </c>
-      <c r="C109" s="94"/>
+      <c r="B109" s="74" t="s">
+        <v>189</v>
+      </c>
+      <c r="C109" s="74"/>
       <c r="D109" s="43"/>
       <c r="E109" s="43"/>
       <c r="F109" s="34" t="s">
@@ -11180,14 +11213,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="110" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A110" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B110" s="94" t="s">
-        <v>190</v>
-      </c>
-      <c r="C110" s="94"/>
+        <v>191</v>
+      </c>
+      <c r="B110" s="74" t="s">
+        <v>189</v>
+      </c>
+      <c r="C110" s="74"/>
       <c r="D110" s="43"/>
       <c r="E110" s="43"/>
       <c r="F110" s="34" t="s">
@@ -11263,14 +11296,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="111" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="111" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A111" s="33" t="s">
-        <v>193</v>
-      </c>
-      <c r="B111" s="94" t="s">
-        <v>190</v>
-      </c>
-      <c r="C111" s="94"/>
+        <v>192</v>
+      </c>
+      <c r="B111" s="74" t="s">
+        <v>189</v>
+      </c>
+      <c r="C111" s="74"/>
       <c r="D111" s="43"/>
       <c r="E111" s="43"/>
       <c r="F111" s="34" t="s">
@@ -11346,14 +11379,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="112" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="112" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A112" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="B112" s="94" t="s">
-        <v>190</v>
-      </c>
-      <c r="C112" s="94"/>
+        <v>193</v>
+      </c>
+      <c r="B112" s="74" t="s">
+        <v>189</v>
+      </c>
+      <c r="C112" s="74"/>
       <c r="D112" s="43"/>
       <c r="E112" s="43"/>
       <c r="F112" s="34" t="s">
@@ -11429,14 +11462,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="113" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A113" s="33" t="s">
-        <v>195</v>
-      </c>
-      <c r="B113" s="94" t="s">
-        <v>190</v>
-      </c>
-      <c r="C113" s="94"/>
+        <v>194</v>
+      </c>
+      <c r="B113" s="74" t="s">
+        <v>189</v>
+      </c>
+      <c r="C113" s="74"/>
       <c r="D113" s="43"/>
       <c r="E113" s="43"/>
       <c r="F113" s="34" t="s">
@@ -11512,14 +11545,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="114" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="114" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A114" s="33" t="s">
-        <v>196</v>
-      </c>
-      <c r="B114" s="94" t="s">
-        <v>190</v>
-      </c>
-      <c r="C114" s="94"/>
+        <v>195</v>
+      </c>
+      <c r="B114" s="74" t="s">
+        <v>189</v>
+      </c>
+      <c r="C114" s="74"/>
       <c r="D114" s="43"/>
       <c r="E114" s="43"/>
       <c r="F114" s="34" t="s">
@@ -11595,14 +11628,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="115" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="115" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A115" s="33" t="s">
+        <v>196</v>
+      </c>
+      <c r="B115" s="73" t="s">
         <v>197</v>
       </c>
-      <c r="B115" s="89" t="s">
-        <v>198</v>
-      </c>
-      <c r="C115" s="89"/>
+      <c r="C115" s="73"/>
       <c r="D115" s="43"/>
       <c r="E115" s="43"/>
       <c r="F115" s="34" t="s">
@@ -11678,14 +11711,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="116" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A116" s="33" t="s">
+        <v>198</v>
+      </c>
+      <c r="B116" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="B116" s="89" t="s">
-        <v>200</v>
-      </c>
-      <c r="C116" s="89"/>
+      <c r="C116" s="73"/>
       <c r="D116" s="43"/>
       <c r="E116" s="43"/>
       <c r="F116" s="34" t="s">
@@ -11761,14 +11794,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="117" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A117" s="33" t="s">
+        <v>200</v>
+      </c>
+      <c r="B117" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="B117" s="89" t="s">
-        <v>202</v>
-      </c>
-      <c r="C117" s="89"/>
+      <c r="C117" s="73"/>
       <c r="D117" s="43"/>
       <c r="E117" s="43"/>
       <c r="F117" s="34" t="s">
@@ -11844,14 +11877,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="118" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="118" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A118" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="B118" s="73" t="s">
         <v>203</v>
       </c>
-      <c r="B118" s="89" t="s">
-        <v>204</v>
-      </c>
-      <c r="C118" s="89"/>
+      <c r="C118" s="73"/>
       <c r="D118" s="43"/>
       <c r="E118" s="43"/>
       <c r="F118" s="34" t="s">
@@ -11927,14 +11960,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="119" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A119" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="B119" s="73" t="s">
         <v>205</v>
       </c>
-      <c r="B119" s="89" t="s">
-        <v>206</v>
-      </c>
-      <c r="C119" s="89"/>
+      <c r="C119" s="73"/>
       <c r="D119" s="43"/>
       <c r="E119" s="43"/>
       <c r="F119" s="34" t="s">
@@ -12010,14 +12043,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="120" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A120" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="B120" s="73" t="s">
         <v>207</v>
       </c>
-      <c r="B120" s="89" t="s">
-        <v>208</v>
-      </c>
-      <c r="C120" s="89"/>
+      <c r="C120" s="73"/>
       <c r="D120" s="43"/>
       <c r="E120" s="43"/>
       <c r="F120" s="34" t="s">
@@ -12093,14 +12126,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="121" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A121" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="B121" s="73" t="s">
         <v>209</v>
       </c>
-      <c r="B121" s="89" t="s">
-        <v>210</v>
-      </c>
-      <c r="C121" s="89"/>
+      <c r="C121" s="73"/>
       <c r="D121" s="43"/>
       <c r="E121" s="43"/>
       <c r="F121" s="34" t="s">
@@ -12176,14 +12209,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="122" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A122" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="B122" s="73" t="s">
         <v>211</v>
       </c>
-      <c r="B122" s="89" t="s">
-        <v>212</v>
-      </c>
-      <c r="C122" s="89"/>
+      <c r="C122" s="73"/>
       <c r="D122" s="43"/>
       <c r="E122" s="43"/>
       <c r="F122" s="34" t="s">
@@ -12259,14 +12292,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="123" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A123" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="B123" s="73" t="s">
         <v>213</v>
       </c>
-      <c r="B123" s="89" t="s">
-        <v>214</v>
-      </c>
-      <c r="C123" s="89"/>
+      <c r="C123" s="73"/>
       <c r="D123" s="43"/>
       <c r="E123" s="43"/>
       <c r="F123" s="34" t="s">
@@ -12342,14 +12375,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="124" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A124" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="B124" s="73" t="s">
         <v>215</v>
       </c>
-      <c r="B124" s="89" t="s">
-        <v>216</v>
-      </c>
-      <c r="C124" s="89"/>
+      <c r="C124" s="73"/>
       <c r="D124" s="43"/>
       <c r="E124" s="43"/>
       <c r="F124" s="34" t="s">
@@ -12425,14 +12458,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="125" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A125" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="B125" s="73" t="s">
         <v>217</v>
       </c>
-      <c r="B125" s="89" t="s">
-        <v>218</v>
-      </c>
-      <c r="C125" s="89"/>
+      <c r="C125" s="73"/>
       <c r="D125" s="43"/>
       <c r="E125" s="43"/>
       <c r="F125" s="34" t="s">
@@ -12508,14 +12541,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="126" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A126" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="B126" s="73" t="s">
         <v>219</v>
       </c>
-      <c r="B126" s="89" t="s">
-        <v>220</v>
-      </c>
-      <c r="C126" s="89"/>
+      <c r="C126" s="73"/>
       <c r="D126" s="43"/>
       <c r="E126" s="43"/>
       <c r="F126" s="34" t="s">
@@ -12591,14 +12624,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="127" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A127" s="33" t="s">
+        <v>220</v>
+      </c>
+      <c r="B127" s="73" t="s">
         <v>221</v>
       </c>
-      <c r="B127" s="89" t="s">
-        <v>222</v>
-      </c>
-      <c r="C127" s="89"/>
+      <c r="C127" s="73"/>
       <c r="D127" s="43"/>
       <c r="E127" s="43"/>
       <c r="F127" s="34" t="s">
@@ -12674,14 +12707,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:30" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="128" spans="1:30" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A128" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="B128" s="73" t="s">
         <v>223</v>
       </c>
-      <c r="B128" s="89" t="s">
-        <v>224</v>
-      </c>
-      <c r="C128" s="89"/>
+      <c r="C128" s="73"/>
       <c r="D128" s="43"/>
       <c r="E128" s="43"/>
       <c r="F128" s="34" t="s">
@@ -12757,14 +12790,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:255" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="129" spans="1:255" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A129" s="33" t="s">
+        <v>224</v>
+      </c>
+      <c r="B129" s="73" t="s">
         <v>225</v>
       </c>
-      <c r="B129" s="89" t="s">
-        <v>226</v>
-      </c>
-      <c r="C129" s="89"/>
+      <c r="C129" s="73"/>
       <c r="D129" s="43"/>
       <c r="E129" s="43"/>
       <c r="F129" s="34" t="s">
@@ -12840,14 +12873,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:255" s="10" customFormat="1" ht="38.5" customHeight="1">
+    <row r="130" spans="1:255" s="10" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A130" s="33" t="s">
+        <v>226</v>
+      </c>
+      <c r="B130" s="73" t="s">
         <v>227</v>
       </c>
-      <c r="B130" s="89" t="s">
-        <v>228</v>
-      </c>
-      <c r="C130" s="89"/>
+      <c r="C130" s="73"/>
       <c r="D130" s="43"/>
       <c r="E130" s="43"/>
       <c r="F130" s="34" t="s">
@@ -12923,14 +12956,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:255" s="47" customFormat="1" ht="38.5" customHeight="1">
+    <row r="131" spans="1:255" s="47" customFormat="1" ht="38.450000000000003" customHeight="1">
       <c r="A131" s="33" t="s">
+        <v>228</v>
+      </c>
+      <c r="B131" s="72" t="s">
         <v>229</v>
       </c>
-      <c r="B131" s="86" t="s">
-        <v>230</v>
-      </c>
-      <c r="C131" s="86"/>
+      <c r="C131" s="72"/>
       <c r="D131" s="34"/>
       <c r="E131" s="34"/>
       <c r="F131" s="34" t="s">
@@ -13234,13 +13267,13 @@
     </row>
     <row r="132" spans="1:255" s="10" customFormat="1">
       <c r="A132" s="48" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B132" s="26"/>
       <c r="C132" s="49"/>
       <c r="D132" s="50"/>
       <c r="F132" s="51" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H132" s="52"/>
       <c r="I132" s="53"/>
@@ -13265,7 +13298,7 @@
     </row>
     <row r="133" spans="1:255" s="10" customFormat="1">
       <c r="A133" s="58" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B133" s="59"/>
       <c r="C133" s="60"/>
@@ -13292,7 +13325,7 @@
     </row>
     <row r="134" spans="1:255" s="10" customFormat="1">
       <c r="A134" s="58" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B134" s="59"/>
       <c r="C134" s="60"/>
@@ -13319,7 +13352,7 @@
     </row>
     <row r="135" spans="1:255" s="10" customFormat="1">
       <c r="A135" s="71" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B135" s="62"/>
       <c r="C135" s="1"/>
@@ -13346,7 +13379,7 @@
     </row>
     <row r="136" spans="1:255" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A136" s="71" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B136" s="62"/>
       <c r="C136" s="1"/>
@@ -13373,7 +13406,7 @@
     </row>
     <row r="137" spans="1:255" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A137" s="58" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B137" s="62"/>
       <c r="C137" s="1"/>
@@ -13400,7 +13433,7 @@
     </row>
     <row r="138" spans="1:255" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A138" s="58" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B138" s="62"/>
       <c r="C138" s="1"/>
@@ -13427,7 +13460,7 @@
     </row>
     <row r="139" spans="1:255" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A139" s="58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B139" s="62"/>
       <c r="C139" s="1"/>
@@ -13454,7 +13487,7 @@
     </row>
     <row r="140" spans="1:255" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A140" s="58" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B140" s="62"/>
       <c r="C140" s="1"/>
@@ -13481,7 +13514,7 @@
     </row>
     <row r="141" spans="1:255" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A141" s="58" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B141" s="62"/>
       <c r="C141" s="1"/>
@@ -13508,7 +13541,7 @@
     </row>
     <row r="142" spans="1:255" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A142" s="58" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B142" s="62"/>
       <c r="C142" s="1"/>
@@ -13535,7 +13568,7 @@
     </row>
     <row r="143" spans="1:255" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A143" s="58" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B143" s="62"/>
       <c r="C143" s="1"/>
@@ -13562,7 +13595,7 @@
     </row>
     <row r="144" spans="1:255">
       <c r="A144" s="71" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B144" s="59"/>
       <c r="C144" s="60"/>
@@ -13585,7 +13618,7 @@
     </row>
     <row r="145" spans="1:46" s="56" customFormat="1" ht="21" customHeight="1">
       <c r="A145" s="71" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B145" s="59"/>
       <c r="C145" s="60"/>
@@ -13612,7 +13645,7 @@
     </row>
     <row r="146" spans="1:46" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A146" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B146" s="66"/>
       <c r="C146" s="67"/>
@@ -13639,7 +13672,7 @@
     </row>
     <row r="147" spans="1:46" s="56" customFormat="1" ht="21" customHeight="1">
       <c r="A147" s="71" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B147" s="59"/>
       <c r="C147" s="60"/>
@@ -13666,7 +13699,7 @@
     </row>
     <row r="148" spans="1:46" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A148" s="71" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B148" s="59"/>
       <c r="C148" s="60"/>
@@ -13693,7 +13726,7 @@
     </row>
     <row r="149" spans="1:46" s="10" customFormat="1" ht="21" customHeight="1">
       <c r="A149" s="71" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B149" s="59"/>
       <c r="C149" s="60"/>
@@ -14222,133 +14255,6 @@
     </row>
   </sheetData>
   <mergeCells count="141">
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A2:U2"/>
     <mergeCell ref="J5:K5"/>
@@ -14363,6 +14269,133 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:S7"/>
     <mergeCell ref="T7:U7"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>